<commit_message>
PF-2242 - View potential partners as a final step of workflows (all) * Adding Taxonomy to the scoring * Giving two setups, one of which shows how multiple sub-scores works
</commit_message>
<xml_diff>
--- a/DesignDocuments/Matchmaker Scoring Example.xlsx
+++ b/DesignDocuments/Matchmaker Scoring Example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stewart.SITKA\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\DesignDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F929D0E-C314-427D-BFE9-B48B6F745E73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A6FE06-D7F5-4913-A098-373441335FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39990" yWindow="7935" windowWidth="23685" windowHeight="14850" xr2:uid="{9BD8518C-54E2-4B55-88C2-B18128FBE1C1}"/>
+    <workbookView xWindow="39930" yWindow="8475" windowWidth="23685" windowHeight="14430" xr2:uid="{9BD8518C-54E2-4B55-88C2-B18128FBE1C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Partner Finder Matchmaker Algorithm sketch</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>* Final Matchmaker Scores are 0.0 to 1.0, with 0 being the lowest quality match, and 1.0 being the best quality match</t>
   </si>
@@ -47,9 +44,6 @@
     <t xml:space="preserve">* There is a cutoff value in the system below which Final Matchmaker Scores won't be displayed, MatchScoreDisplayCutoff. Right now this is 0.5. </t>
   </si>
   <si>
-    <t>v1.0</t>
-  </si>
-  <si>
     <t>Taxonomy</t>
   </si>
   <si>
@@ -105,6 +99,36 @@
   </si>
   <si>
     <t>(Explanation of yyy SubScore could go here.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Matches Leaf</t>
+  </si>
+  <si>
+    <t>Matches Leaf on Branch</t>
+  </si>
+  <si>
+    <t>Matches Leaf on Trunk</t>
+  </si>
+  <si>
+    <t>Any Match</t>
+  </si>
+  <si>
+    <t>Taxonomy SubScore</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>If/when we have multiple sub-scores:</t>
+  </si>
+  <si>
+    <t>As implemented 8/13/2020 (only one subscore so far):</t>
+  </si>
+  <si>
+    <t>Partner Finder Matchmaker Algorithm Worksheet</t>
   </si>
 </sst>
 </file>
@@ -113,7 +137,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -194,8 +218,8 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -511,15 +535,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9802303-EF3C-48CA-9900-5C41435FF356}">
-  <dimension ref="A2:H33"/>
+  <dimension ref="A2:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -528,83 +552,89 @@
   <sheetData>
     <row r="2" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B3" s="5">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="C3" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.72916666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="8">
-        <v>0.82</v>
+        <f>+$B$40</f>
+        <v>1</v>
       </c>
       <c r="D13" s="9">
         <f>+C13*$H$15</f>
-        <v>0.20499999999999999</v>
+        <v>0.25</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H13">
-        <f>COUNT(C13:C19)</f>
+        <f>COUNT(C13:C21)</f>
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C14" s="8">
-        <v>0.61</v>
+        <v>0.1</v>
       </c>
       <c r="D14" s="9">
         <f>+C14*$H$15</f>
-        <v>0.1525</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H14" s="7">
         <v>1</v>
@@ -612,17 +642,17 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" s="8">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="D15" s="9">
         <f>+C15*$H$15</f>
-        <v>5.2499999999999998E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H15">
         <f>+H14/H13</f>
@@ -631,59 +661,179 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" s="8">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="D16" s="9">
         <f>+C16*$H$15</f>
-        <v>0.17499999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="10">
+        <f>SUM(D13:D16)</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="10">
-        <f>SUM(D13:D19)</f>
-        <v>0.58499999999999996</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="8">
+        <f>+$B$40</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="9">
+        <f>+C23*$H$25</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <f>COUNT(C23:C32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="G24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="10">
+        <f>SUM(D23)</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25">
+        <f>+H24/H23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" t="b">
+        <f>OR(B34,B35,B36)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="8">
+        <f>IF(B38, 1, 0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+    <row r="46" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A46" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PF-2238 - Edit Org profile (Keywords) * Updating the Matchmaker Scoring Example Excel sheet. (Is this actually helping anyone?) * Decreasing the MatchScoreDisplayCutoff so it shows all results currently. If it was above .3, that would mean we were requiring that a project/org hit on *more* than one sub-score, which seems overly restrictive to me for the moment. Probably this value needs to be admin-configurable and devs can step out of this debate as much as possible.
</commit_message>
<xml_diff>
--- a/DesignDocuments/Matchmaker Scoring Example.xlsx
+++ b/DesignDocuments/Matchmaker Scoring Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\DesignDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A6FE06-D7F5-4913-A098-373441335FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0F6261-DE45-4B77-B253-0734644C0088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39930" yWindow="8475" windowWidth="23685" windowHeight="14430" xr2:uid="{9BD8518C-54E2-4B55-88C2-B18128FBE1C1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>* Final Matchmaker Scores are 0.0 to 1.0, with 0 being the lowest quality match, and 1.0 being the best quality match</t>
   </si>
@@ -41,21 +41,9 @@
     <t>* Final Matchmaker Scores are bidirectional, so a fitness score of 0.85 for Organization =&gt; Project is also a fitness score of 0.85 Project =&gt; Organization</t>
   </si>
   <si>
-    <t xml:space="preserve">* There is a cutoff value in the system below which Final Matchmaker Scores won't be displayed, MatchScoreDisplayCutoff. Right now this is 0.5. </t>
-  </si>
-  <si>
     <t>Taxonomy</t>
   </si>
   <si>
-    <t>xxx</t>
-  </si>
-  <si>
-    <t>yyy</t>
-  </si>
-  <si>
-    <t>zzz</t>
-  </si>
-  <si>
     <t>* Final Matchmaker Scores are composed of SubScores, which also range from 0.0 to 1.0. They are summed as follows:</t>
   </si>
   <si>
@@ -86,21 +74,6 @@
     <t>Taxonomy SubScore:</t>
   </si>
   <si>
-    <t>(Explanation of Taxonomy SubScore could go here.)</t>
-  </si>
-  <si>
-    <t>xxx SubScore:</t>
-  </si>
-  <si>
-    <t>(Explanation of xxx SubScore could go here.)</t>
-  </si>
-  <si>
-    <t>yyy SubScore:</t>
-  </si>
-  <si>
-    <t>(Explanation of yyy SubScore could go here.)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -119,27 +92,61 @@
     <t>Taxonomy SubScore</t>
   </si>
   <si>
-    <t>v1.1</t>
-  </si>
-  <si>
     <t>If/when we have multiple sub-scores:</t>
   </si>
   <si>
-    <t>As implemented 8/13/2020 (only one subscore so far):</t>
-  </si>
-  <si>
     <t>Partner Finder Matchmaker Algorithm Worksheet</t>
+  </si>
+  <si>
+    <t>Area of Interest</t>
+  </si>
+  <si>
+    <t>Matchmaker Keyword</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>Area of Interest SubScore:</t>
+  </si>
+  <si>
+    <t>Simple Location Intersection</t>
+  </si>
+  <si>
+    <t>Detailed Location Intersection</t>
+  </si>
+  <si>
+    <t>Geospatial Area Intersection</t>
+  </si>
+  <si>
+    <t>Area of Interest SubScore</t>
+  </si>
+  <si>
+    <t>Matchmaker Keyword SubScore:</t>
+  </si>
+  <si>
+    <t>Keyword match on Project Name</t>
+  </si>
+  <si>
+    <t>Keyword match on Project Description</t>
+  </si>
+  <si>
+    <t>Matchmaker Keyword SubScore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* There is a cutoff value in the system below which Final Matchmaker Scores won't be displayed, MatchScoreDisplayCutoff. Right now this is 0.2. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,14 +186,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -220,7 +219,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,16 +535,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9802303-EF3C-48CA-9900-5C41435FF356}">
-  <dimension ref="A2:H47"/>
+  <dimension ref="A2:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
@@ -552,18 +552,18 @@
   <sheetData>
     <row r="2" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B3" s="5">
-        <v>44056</v>
+        <v>44090</v>
       </c>
       <c r="C3" s="6">
-        <v>0.72916666666666663</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -578,63 +578,64 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="8">
-        <f>+$B$40</f>
+        <f>+$B$30</f>
         <v>1</v>
       </c>
       <c r="D13" s="9">
         <f>+C13*$H$15</f>
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H13">
-        <f>COUNT(C13:C21)</f>
-        <v>4</v>
+        <f>COUNT(C13:C16)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C14" s="8">
-        <v>0.1</v>
+        <f>+B38</f>
+        <v>1</v>
       </c>
       <c r="D14" s="9">
         <f>+C14*$H$15</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H14" s="7">
         <v>1</v>
@@ -642,198 +643,164 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C15" s="8">
-        <v>0.2</v>
+        <f>+B46</f>
+        <v>0</v>
       </c>
       <c r="D15" s="9">
         <f>+C15*$H$15</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="12">
+        <f>+H14/H13</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="10">
+        <f>SUM(D13:D15)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H15">
-        <f>+H14/H13</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="D16" s="9">
-        <f>+C16*$H$15</f>
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="10">
-        <f>SUM(D13:D16)</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1" t="s">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="8">
-        <f>+$B$40</f>
+      <c r="B25" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="9">
-        <f>+C23*$H$25</f>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="b">
+        <f>OR(B24,B25,B26)</f>
         <v>1</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23">
-        <f>COUNT(C23:C32)</f>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="11">
+        <f>IF(B28, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="G24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="10">
-        <f>SUM(D23)</f>
-        <v>1</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25">
-        <f>+H24/H23</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>22</v>
+    <row r="32" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" t="b">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="B34" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" t="b">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="B35" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" t="b">
+        <v>27</v>
+      </c>
+      <c r="B36" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" t="b">
-        <f>OR(B34,B35,B36)</f>
+      <c r="A38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="11">
+        <f>MAX(B34:B36)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B40" s="8">
-        <f>IF(B38, 1, 0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
-        <v>18</v>
+    <row r="41" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>21</v>
+      <c r="A43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="11">
+        <f>MAX(B43:B44)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PF-2235 Edit org profile (Classifications) * adjust algorithm to include classifications
</commit_message>
<xml_diff>
--- a/DesignDocuments/Matchmaker Scoring Example.xlsx
+++ b/DesignDocuments/Matchmaker Scoring Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\sitkatech\projectfirma\DesignDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0F6261-DE45-4B77-B253-0734644C0088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD3F783-3E8A-4970-A5D6-CE46194223D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39930" yWindow="8475" windowWidth="23685" windowHeight="14430" xr2:uid="{9BD8518C-54E2-4B55-88C2-B18128FBE1C1}"/>
+    <workbookView xWindow="2550" yWindow="5040" windowWidth="36705" windowHeight="17280" xr2:uid="{9BD8518C-54E2-4B55-88C2-B18128FBE1C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>* Final Matchmaker Scores are 0.0 to 1.0, with 0 being the lowest quality match, and 1.0 being the best quality match</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t xml:space="preserve">* There is a cutoff value in the system below which Final Matchmaker Scores won't be displayed, MatchScoreDisplayCutoff. Right now this is 0.2. </t>
+  </si>
+  <si>
+    <t>Matchmaker Classifications SubScore:</t>
+  </si>
+  <si>
+    <t>Classification match between project and organization</t>
+  </si>
+  <si>
+    <t>Matchmaker Classifications SubScore</t>
+  </si>
+  <si>
+    <t>Classifications</t>
   </si>
 </sst>
 </file>
@@ -144,7 +156,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -220,7 +232,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9802303-EF3C-48CA-9900-5C41435FF356}">
-  <dimension ref="A2:H46"/>
+  <dimension ref="A2:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,14 +624,13 @@
       </c>
       <c r="D13" s="9">
         <f>+C13*$H$15</f>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H13">
-        <f>COUNT(C13:C16)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -632,7 +643,7 @@
       </c>
       <c r="D14" s="9">
         <f>+C14*$H$15</f>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>7</v>
@@ -658,12 +669,21 @@
       </c>
       <c r="H15" s="12">
         <f>+H14/H13</f>
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="8">
+        <f>B53</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="9">
+        <f>+C16*$H$15</f>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
@@ -671,8 +691,8 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="10">
-        <f>SUM(D13:D15)</f>
-        <v>0.66666666666666663</v>
+        <f>SUM(D13:D16)</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -801,6 +821,28 @@
       <c r="B46" s="11">
         <f>MAX(B43:B44)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="11">
+        <f>B51</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>